<commit_message>
FINAL (HOPEFULLY HOLY SHIT)
</commit_message>
<xml_diff>
--- a/G431_MCU_Board/Project Outputs for G431_MCU_Board/BOM/Bill of Materials-G431_MCU_Board.xlsx
+++ b/G431_MCU_Board/Project Outputs for G431_MCU_Board/BOM/Bill of Materials-G431_MCU_Board.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\shared\Waterloop\altium\electrical-mcu\G431\G431_MCU_Board\Project Outputs for G431_MCU_Board\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5F70444C-EE30-4527-8BAD-2EE83879372A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{CD97B1C9-EA2F-4D3A-A8DC-7F1179896DA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3120" yWindow="3120" windowWidth="21600" windowHeight="11385" xr2:uid="{71C96102-B9DB-4550-BED0-0643712E5710}"/>
+    <workbookView xWindow="1950" yWindow="1950" windowWidth="21600" windowHeight="11385" xr2:uid="{2C0AF6EE-B90F-4A31-9777-F38D661367C0}"/>
   </bookViews>
   <sheets>
     <sheet name="Bill of Materials-G431_MCU_Boar" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="94">
   <si>
     <t>Designator</t>
   </si>
@@ -64,49 +64,55 @@
     <t>Quantity</t>
   </si>
   <si>
-    <t>C1, C3, C6, C7, C8, C14, C15, C16, C17, C18</t>
+    <t>C1, C5, C6, C7, C13, C14, C15, C16, C17</t>
   </si>
   <si>
     <t>100nF</t>
   </si>
   <si>
+    <t>0603 - Capacitor, 0805 - Capacitor</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>C2</t>
+  </si>
+  <si>
+    <t>DNP</t>
+  </si>
+  <si>
     <t>0603 - Capacitor</t>
   </si>
   <si>
-    <t/>
-  </si>
-  <si>
-    <t>C2</t>
-  </si>
-  <si>
-    <t>DNP</t>
+    <t>C3</t>
+  </si>
+  <si>
+    <t>10nF</t>
   </si>
   <si>
     <t>C4</t>
   </si>
   <si>
-    <t>10nF</t>
-  </si>
-  <si>
-    <t>C5</t>
-  </si>
-  <si>
     <t>1uF</t>
   </si>
   <si>
-    <t>C9, C10</t>
+    <t>C8, C9</t>
   </si>
   <si>
     <t>32pF</t>
   </si>
   <si>
-    <t>C11, C13</t>
+    <t>C10, C12</t>
   </si>
   <si>
     <t>10uF</t>
   </si>
   <si>
-    <t>C12</t>
+    <t>0805 - Capacitor</t>
+  </si>
+  <si>
+    <t>C11</t>
   </si>
   <si>
     <t>22uF</t>
@@ -196,21 +202,21 @@
     <t>230</t>
   </si>
   <si>
-    <t>R8, R9, R10, R11</t>
+    <t>R8, R9, R10</t>
   </si>
   <si>
     <t>1k</t>
   </si>
   <si>
+    <t>R11</t>
+  </si>
+  <si>
+    <t>350</t>
+  </si>
+  <si>
     <t>R12</t>
   </si>
   <si>
-    <t>350</t>
-  </si>
-  <si>
-    <t>R13</t>
-  </si>
-  <si>
     <t>150</t>
   </si>
   <si>
@@ -223,19 +229,13 @@
     <t>U1</t>
   </si>
   <si>
-    <t>SOT95P285X140-3N</t>
-  </si>
-  <si>
-    <t>Diodes Inc.</t>
-  </si>
-  <si>
-    <t>AP1704DWG-7</t>
-  </si>
-  <si>
-    <t>Diji-Key</t>
-  </si>
-  <si>
-    <t>AP1704DWGDITR-ND</t>
+    <t>FP-SOT143-4-MFG</t>
+  </si>
+  <si>
+    <t>STMicroelectronics</t>
+  </si>
+  <si>
+    <t>STM811MW16F</t>
   </si>
   <si>
     <t>U2</t>
@@ -695,7 +695,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB1A5AF1-132B-429F-8BF8-B8660D086365}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1ADCE0FE-4AD5-46E6-9872-B5CD3E03F3E6}">
   <dimension ref="A1:H32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
@@ -756,7 +756,7 @@
         <v>11</v>
       </c>
       <c r="H2" s="1">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -767,7 +767,7 @@
         <v>13</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
@@ -779,13 +779,13 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>14</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>10</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
@@ -797,13 +797,13 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
@@ -815,13 +815,13 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>11</v>
@@ -841,13 +841,13 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>10</v>
+        <v>23</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>11</v>
@@ -867,13 +867,13 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B8" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8" s="2" t="s">
         <v>23</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>10</v>
       </c>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
@@ -885,23 +885,23 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B9" s="1"/>
       <c r="C9" s="2" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="H9" s="1">
         <v>1</v>
@@ -909,23 +909,23 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B10" s="1"/>
       <c r="C10" s="2" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="H10" s="1">
         <v>1</v>
@@ -933,11 +933,11 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B11" s="1"/>
       <c r="C11" s="2" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
@@ -949,23 +949,23 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B12" s="1"/>
       <c r="C12" s="2" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="H12" s="1">
         <v>1</v>
@@ -973,11 +973,11 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B13" s="1"/>
       <c r="C13" s="2" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
@@ -989,11 +989,11 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B14" s="1"/>
       <c r="C14" s="2" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
@@ -1005,11 +1005,11 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B15" s="1"/>
       <c r="C15" s="2" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
@@ -1021,11 +1021,11 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B16" s="1"/>
       <c r="C16" s="2" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
@@ -1037,11 +1037,11 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B17" s="1"/>
       <c r="C17" s="2" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
@@ -1053,13 +1053,13 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C18" s="2" t="s">
         <v>47</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>45</v>
       </c>
       <c r="D18" s="2" t="s">
         <v>11</v>
@@ -1079,13 +1079,13 @@
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>13</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
@@ -1097,13 +1097,13 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B20" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C20" s="2" t="s">
         <v>51</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>49</v>
       </c>
       <c r="D20" s="2" t="s">
         <v>11</v>
@@ -1123,13 +1123,13 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="D21" s="2" t="s">
         <v>11</v>
@@ -1144,18 +1144,18 @@
         <v>11</v>
       </c>
       <c r="H21" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
@@ -1167,13 +1167,13 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
@@ -1185,11 +1185,11 @@
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="B24" s="1"/>
       <c r="C24" s="2" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="D24" s="1"/>
       <c r="E24" s="1"/>
@@ -1201,24 +1201,20 @@
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="B25" s="1"/>
       <c r="C25" s="2" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="F25" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="G25" s="2" t="s">
         <v>65</v>
       </c>
+      <c r="F25" s="1"/>
+      <c r="G25" s="1"/>
       <c r="H25" s="1">
         <v>1</v>
       </c>

</xml_diff>